<commit_message>
update to v1.8, but some functions breaks... ignore them temporarily
</commit_message>
<xml_diff>
--- a/settings/en/template_blueprints.xlsx
+++ b/settings/en/template_blueprints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\game_mod\against_storm\export_analysis\settings\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E9F8FA-D490-4875-A4A2-01B4E9F256BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D898EA11-93CA-472F-932C-458A5D30C1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,11 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
-  <si>
-    <t>0.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="99">
   <si>
     <t>https://github.com/Forwindzz/ATSUnpackToExcel</t>
   </si>
@@ -417,12 +413,28 @@
     <t>Final Options the player will see</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>m0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update to 1.6 game ver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m0.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update to 1.8 game ver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,6 +501,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -596,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -646,6 +666,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -928,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -945,278 +966,278 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="A1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H3">
-        <v>1.4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>0</v>
+        <v>1.8</v>
+      </c>
+      <c r="I3">
+        <v>0.4</v>
       </c>
       <c r="J3" s="1">
-        <v>45598</v>
+        <v>45871</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1225,18 +1246,18 @@
         <v>0</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1245,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1253,7 +1274,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -1262,10 +1283,10 @@
         <v>0</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -1273,7 +1294,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1282,10 +1303,10 @@
         <v>1</v>
       </c>
       <c r="G49" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H49" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -1293,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D50">
         <v>3</v>
@@ -1302,13 +1323,13 @@
         <v>0</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -1316,7 +1337,7 @@
         <v>3</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1325,13 +1346,13 @@
         <v>1</v>
       </c>
       <c r="G51" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -1339,7 +1360,7 @@
         <v>4</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D52">
         <v>3</v>
@@ -1348,27 +1369,27 @@
         <v>1</v>
       </c>
       <c r="G52" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53">
         <v>4</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -1377,61 +1398,81 @@
         <v>2</v>
       </c>
       <c r="G53" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H53" s="6" t="s">
+      <c r="J53" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1473,22 +1514,22 @@
   <sheetData>
     <row r="1" spans="1:29" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1496,10 +1537,10 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1509,16 +1550,16 @@
         <v>0</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="G8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -1526,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1536,7 +1577,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -1546,15 +1587,15 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="F11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -1562,15 +1603,15 @@
         <v>12</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="F12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -1578,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1606,7 +1647,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="I14" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="16">
         <v>17</v>
@@ -1686,7 +1727,7 @@
       <c r="Z15" s="18"/>
       <c r="AA15" s="18"/>
       <c r="AB15" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC15" s="9"/>
     </row>
@@ -1710,7 +1751,7 @@
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
       <c r="AA16" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB16" s="10"/>
       <c r="AC16" s="10"/>
@@ -1728,17 +1769,17 @@
       <c r="R17" s="20"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V17" s="10"/>
       <c r="W17" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X17" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
@@ -1759,7 +1800,7 @@
       <c r="R18" s="20"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
@@ -1781,7 +1822,7 @@
       <c r="P19" s="20"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -1804,7 +1845,7 @@
       <c r="N20" s="20"/>
       <c r="O20" s="10"/>
       <c r="P20" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
@@ -1827,7 +1868,7 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
@@ -1873,18 +1914,18 @@
     </row>
     <row r="23" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F23" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F24" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="6:29" x14ac:dyDescent="0.2">
@@ -1910,7 +1951,7 @@
     </row>
     <row r="26" spans="6:29" x14ac:dyDescent="0.2">
       <c r="I26" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J26" s="16">
         <v>17</v>
@@ -1985,7 +2026,7 @@
       <c r="Z27" s="18"/>
       <c r="AA27" s="18"/>
       <c r="AB27" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="6:29" x14ac:dyDescent="0.2">
@@ -2006,7 +2047,7 @@
       <c r="Y28" s="10"/>
       <c r="Z28" s="10"/>
       <c r="AA28" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="6:29" x14ac:dyDescent="0.2">
@@ -2021,12 +2062,12 @@
       <c r="Q29" s="20"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
       <c r="W29" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y29" s="10"/>
       <c r="Z29" s="10"/>
@@ -2044,7 +2085,7 @@
       <c r="Q30" s="19"/>
       <c r="S30" s="10"/>
       <c r="T30" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U30" s="10"/>
       <c r="W30" s="10"/>
@@ -2063,7 +2104,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
       <c r="Q31" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
@@ -2104,18 +2145,18 @@
     </row>
     <row r="34" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F34" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F35" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="6:29" x14ac:dyDescent="0.2">
@@ -2143,7 +2184,7 @@
     </row>
     <row r="37" spans="6:29" x14ac:dyDescent="0.2">
       <c r="I37" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
@@ -2215,7 +2256,7 @@
       <c r="Z38" s="18"/>
       <c r="AA38" s="18"/>
       <c r="AB38" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC38" s="9"/>
     </row>
@@ -2238,7 +2279,7 @@
       <c r="Y39" s="10"/>
       <c r="Z39" s="10"/>
       <c r="AA39" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB39" s="10"/>
       <c r="AC39" s="10"/>
@@ -2256,13 +2297,13 @@
       <c r="S40" s="20"/>
       <c r="T40" s="10"/>
       <c r="U40" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X40" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y40" s="10"/>
       <c r="Z40" s="10"/>
@@ -2283,7 +2324,7 @@
       <c r="S41" s="20"/>
       <c r="T41" s="10"/>
       <c r="U41" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V41" s="10"/>
       <c r="W41" s="10"/>
@@ -2306,7 +2347,7 @@
       <c r="Q42" s="20"/>
       <c r="R42" s="10"/>
       <c r="S42" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T42" s="10"/>
       <c r="U42" s="10"/>
@@ -2329,7 +2370,7 @@
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
       <c r="Q43" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
@@ -2372,18 +2413,18 @@
     </row>
     <row r="45" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F45" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="6:29" x14ac:dyDescent="0.2">
       <c r="F46" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="6:29" x14ac:dyDescent="0.2">
@@ -2409,7 +2450,7 @@
     </row>
     <row r="48" spans="6:29" x14ac:dyDescent="0.2">
       <c r="I48" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J48" s="16"/>
       <c r="K48" s="16"/>
@@ -2476,7 +2517,7 @@
       <c r="Z49" s="18"/>
       <c r="AA49" s="18"/>
       <c r="AB49" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="9:28" x14ac:dyDescent="0.2">
@@ -2495,7 +2536,7 @@
       <c r="Y50" s="10"/>
       <c r="Z50" s="10"/>
       <c r="AA50" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="9:28" x14ac:dyDescent="0.2">
@@ -2508,14 +2549,14 @@
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
       <c r="T51" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V51" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W51" s="10"/>
       <c r="X51" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y51" s="10"/>
       <c r="Z51" s="10"/>
@@ -2531,7 +2572,7 @@
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
       <c r="T52" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U52" s="10"/>
       <c r="V52" s="10"/>

</xml_diff>